<commit_message>
Updated syntax for Obsidian aliases
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/z3534868/GitHub/xls2md/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1407A94-6B25-B141-978C-B30EA085DA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72539E53-A669-8F4A-9444-A0C3C1DE3803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -25,15 +38,9 @@
     <t>ID</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
-    <t>class</t>
-  </si>
-  <si>
     <t>z1111111</t>
   </si>
   <si>
@@ -59,6 +66,12 @@
   </si>
   <si>
     <t>m.thatcher@student.email.com</t>
+  </si>
+  <si>
+    <t>alias</t>
+  </si>
+  <si>
+    <t>classID</t>
   </si>
 </sst>
 </file>
@@ -428,7 +441,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -438,24 +451,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>10101</v>
@@ -463,13 +476,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>10102</v>
@@ -477,13 +490,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>10103</v>

</xml_diff>